<commit_message>
Master Project Start on Github
warmup app functional, some styling, project stable, documentation up to
date
</commit_message>
<xml_diff>
--- a/Capstone/Documentation/Weekly Time Tracker.xlsx
+++ b/Capstone/Documentation/Weekly Time Tracker.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="20">
   <si>
     <t>WEEKLY TIME TRACKER</t>
   </si>
@@ -70,6 +70,12 @@
   </si>
   <si>
     <t>Tuesday</t>
+  </si>
+  <si>
+    <t>Work Day</t>
+  </si>
+  <si>
+    <t>Scott McNulty</t>
   </si>
 </sst>
 </file>
@@ -226,7 +232,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -268,6 +274,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -575,7 +584,7 @@
   <dimension ref="A1:H49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -591,8 +600,17 @@
         <v>0</v>
       </c>
       <c r="C1" s="3"/>
+      <c r="D1" s="16" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D2" s="1"/>
     </row>
     <row r="3" spans="1:8" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D3" s="16" t="s">
+        <v>18</v>
+      </c>
       <c r="H3" s="2" t="s">
         <v>16</v>
       </c>
@@ -731,11 +749,15 @@
       <c r="E11" s="12">
         <v>3</v>
       </c>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
+      <c r="F11" s="12">
+        <v>5</v>
+      </c>
+      <c r="G11" s="12">
+        <v>2</v>
+      </c>
       <c r="H11" s="15">
         <f>SUM(A11:G11)</f>
-        <v>11</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -795,29 +817,29 @@
     </row>
     <row r="16" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="11">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B16" s="12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C16" s="12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D16" s="12">
         <v>0</v>
       </c>
       <c r="E16" s="12">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F16" s="12">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G16" s="12">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="H16" s="15">
         <f>SUM(A16:G16)</f>
-        <v>0</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
More work on interval branch
+updated time sheet
</commit_message>
<xml_diff>
--- a/Capstone/Documentation/Weekly Time Tracker.xlsx
+++ b/Capstone/Documentation/Weekly Time Tracker.xlsx
@@ -12,11 +12,12 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="21">
   <si>
     <t>WEEKLY TIME TRACKER</t>
   </si>
@@ -76,6 +77,9 @@
   </si>
   <si>
     <t>Scott McNulty</t>
+  </si>
+  <si>
+    <t>Sleep study</t>
   </si>
 </sst>
 </file>
@@ -232,7 +236,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -277,6 +281,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -584,7 +591,7 @@
   <dimension ref="A1:H49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+      <selection activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -741,7 +748,7 @@
         <v>3</v>
       </c>
       <c r="C11" s="12">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D11" s="12">
         <v>0</v>
@@ -750,14 +757,14 @@
         <v>3</v>
       </c>
       <c r="F11" s="12">
+        <v>2</v>
+      </c>
+      <c r="G11" s="12">
         <v>5</v>
-      </c>
-      <c r="G11" s="12">
-        <v>2</v>
       </c>
       <c r="H11" s="15">
         <f>SUM(A11:G11)</f>
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -786,7 +793,9 @@
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
+      <c r="E14" s="17" t="s">
+        <v>20</v>
+      </c>
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
       <c r="H14" s="14"/>
@@ -820,7 +829,7 @@
         <v>2</v>
       </c>
       <c r="B16" s="12">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C16" s="12">
         <v>2</v>
@@ -829,13 +838,13 @@
         <v>0</v>
       </c>
       <c r="E16" s="12">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F16" s="12">
         <v>3</v>
       </c>
       <c r="G16" s="12">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H16" s="15">
         <f>SUM(A16:G16)</f>
@@ -899,29 +908,29 @@
     </row>
     <row r="21" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="11">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B21" s="12">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C21" s="12">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D21" s="12">
         <v>0</v>
       </c>
       <c r="E21" s="12">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F21" s="12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G21" s="12">
-        <v>0</v>
-      </c>
-      <c r="H21" s="15">
+        <v>3</v>
+      </c>
+      <c r="H21" s="13">
         <f>SUM(A21:G21)</f>
-        <v>0</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -981,29 +990,29 @@
     </row>
     <row r="26" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="11">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B26" s="12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C26" s="12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D26" s="12">
         <v>0</v>
       </c>
       <c r="E26" s="12">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F26" s="12">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G26" s="12">
-        <v>0</v>
-      </c>
-      <c r="H26" s="15">
+        <v>3</v>
+      </c>
+      <c r="H26" s="13">
         <f>SUM(A26:G26)</f>
-        <v>0</v>
+        <v>17</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -1063,29 +1072,29 @@
     </row>
     <row r="31" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="11">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B31" s="12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C31" s="12">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D31" s="12">
         <v>0</v>
       </c>
       <c r="E31" s="12">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F31" s="12">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G31" s="12">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="H31" s="15">
         <f>SUM(A31:G31)</f>
-        <v>0</v>
+        <v>23</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>